<commit_message>
some changes in excel sheets
</commit_message>
<xml_diff>
--- a/excel_sheets/details.xlsx
+++ b/excel_sheets/details.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects_withD\spo2_webInterface\Spo2_new\excel_sheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\disha\Desktop\Competitions\SPO2_cam\Spo2_new\excel_sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5BFABB2-819B-4A07-B3BC-526174B516B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF74DB92-7587-4650-AF7D-1523D1350664}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9480" yWindow="300" windowWidth="13560" windowHeight="10668" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,18 +39,6 @@
     <t>Job</t>
   </si>
   <si>
-    <t>sachin</t>
-  </si>
-  <si>
-    <t>satvik</t>
-  </si>
-  <si>
-    <t>dishant</t>
-  </si>
-  <si>
-    <t>sania</t>
-  </si>
-  <si>
     <t>Software Engineer</t>
   </si>
   <si>
@@ -66,13 +54,25 @@
     <t>110/ Pinnecal High, Juhu, Mumbai</t>
   </si>
   <si>
-    <t>802/ Gunjan nagar/ Andheri , Mumabai</t>
-  </si>
-  <si>
     <t>HR</t>
   </si>
   <si>
     <t>Team Lead</t>
+  </si>
+  <si>
+    <t>802/ Gunjan nagar/ Andheri , Mumbai</t>
+  </si>
+  <si>
+    <t>Sachin</t>
+  </si>
+  <si>
+    <t>Satvik</t>
+  </si>
+  <si>
+    <t>Sania</t>
+  </si>
+  <si>
+    <t>Dishant</t>
   </si>
 </sst>
 </file>
@@ -393,13 +393,15 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="26.44140625" customWidth="1"/>
-    <col min="4" max="4" width="19.5546875" customWidth="1"/>
+    <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -421,13 +423,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -435,13 +437,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -449,13 +451,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -463,13 +465,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed auto, added trainer in gui
</commit_message>
<xml_diff>
--- a/excel_sheets/details.xlsx
+++ b/excel_sheets/details.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects_withD\spo2_webInterface\Spo2_new\excel_sheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Codes\Project\SPO2\Spo2_new\excel_sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DD1C49E-6FB2-4C02-A79E-73F017ABC2EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{999D4486-EE60-4319-A429-1233FBF2CBF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2292" windowWidth="13560" windowHeight="10668" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Sr. No</t>
   </si>
@@ -73,6 +73,15 @@
   </si>
   <si>
     <t>dishant</t>
+  </si>
+  <si>
+    <t>soham</t>
+  </si>
+  <si>
+    <t>202/Ring city road, Bandra,Mumbai</t>
+  </si>
+  <si>
+    <t>Deployment</t>
   </si>
 </sst>
 </file>
@@ -390,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -474,6 +483,20 @@
         <v>10</v>
       </c>
     </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
changed sr_no to face_ID
</commit_message>
<xml_diff>
--- a/excel_sheets/details.xlsx
+++ b/excel_sheets/details.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Codes\Project\SPO2\Spo2_new\excel_sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{999D4486-EE60-4319-A429-1233FBF2CBF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{593DD27D-946D-43D8-9103-7BE7F1A307B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,9 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
-    <t>Sr. No</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -82,6 +79,9 @@
   </si>
   <si>
     <t>Deployment</t>
+  </si>
+  <si>
+    <t>Face_ID</t>
   </si>
 </sst>
 </file>
@@ -402,7 +402,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -415,16 +415,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -432,13 +432,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -446,13 +446,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
         <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -460,13 +460,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
         <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -474,13 +474,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -488,13 +488,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
         <v>16</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>17</v>
-      </c>
-      <c r="D6" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>